<commit_message>
for loop instead of search nearby
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\ScaryFlock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C0F4320-83C6-4B13-AE9C-9C93C738A6A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B19146F-2C3F-4695-AE7D-0EB7EE4264E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A30AFCFF-D501-43E3-B0A8-D3BB1839827C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>default</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>10 fps</t>
+  </si>
+  <si>
+    <t>For Loop instead of circle collider</t>
   </si>
 </sst>
 </file>
@@ -147,11 +150,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Update</a:t>
+              <a:t>Performance Around</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Every Frame Vs. Random Update</a:t>
+              <a:t> Checking for Nearby Agents</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -259,7 +262,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -288,10 +291,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2000</c:v>
                 </c:pt>
@@ -349,7 +352,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$9</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -378,10 +381,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2500</c:v>
                 </c:pt>
@@ -409,6 +412,96 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-12A5-445A-9F28-F14E8EBC8F10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>For Loop instead of circle collider</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>70 fps</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60 fps</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50 fps</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40 fps</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30 fps</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20 fps</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10 fps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8EDB-4F59-A6E0-59D7328B34C6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1148,16 +1241,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>962024</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1482,26 +1575,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6AEB0EF-50E8-42FA-B9F7-DABF9F3A240C}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1511,8 +1608,11 @@
       <c r="C2">
         <v>2500</v>
       </c>
+      <c r="D2">
+        <v>175</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1522,8 +1622,11 @@
       <c r="C3">
         <v>3100</v>
       </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1533,8 +1636,11 @@
       <c r="C4">
         <v>3800</v>
       </c>
+      <c r="D4">
+        <v>225</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1544,8 +1650,11 @@
       <c r="C5">
         <v>4800</v>
       </c>
+      <c r="D5">
+        <v>250</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1555,8 +1664,11 @@
       <c r="C6">
         <v>6400</v>
       </c>
+      <c r="D6">
+        <v>275</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1566,8 +1678,11 @@
       <c r="C7">
         <v>9400</v>
       </c>
+      <c r="D7">
+        <v>350</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1576,6 +1691,9 @@
       </c>
       <c r="C8">
         <v>17600</v>
+      </c>
+      <c r="D8">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>